<commit_message>
Added Staff and Admin files. Updated tables with new table query for system logs, added system logs to the populateTestData file, added new table to temporaryData named system_logs.
</commit_message>
<xml_diff>
--- a/backend/temporaryData.xlsx
+++ b/backend/temporaryData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracenguyen/Documents/USF/USF Fall 24/SWE/eduPortal/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokt\Desktop\bloop2\eduPortal\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B407009-A007-6046-86F4-4DA6A40597F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242AE6FB-8150-403A-AD19-395266BEE05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="2200" windowWidth="28040" windowHeight="17440" firstSheet="4" activeTab="4" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="9" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
   </bookViews>
   <sheets>
     <sheet name="student_data" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="taken_data" sheetId="7" r:id="rId7"/>
     <sheet name="major_data" sheetId="8" r:id="rId8"/>
     <sheet name="departmentid" sheetId="9" r:id="rId9"/>
+    <sheet name="system_logs" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -296,6 +297,69 @@
   </si>
   <si>
     <t>ENB</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>operation_type</t>
+  </si>
+  <si>
+    <t>table_name</t>
+  </si>
+  <si>
+    <t>affected_data</t>
+  </si>
+  <si>
+    <t>old_value</t>
+  </si>
+  <si>
+    <t>new_value</t>
+  </si>
+  <si>
+    <t>operation_timestamp</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>WRITE</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>Added course_id=201 to semester=Fall</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Course created</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>READ</t>
+  </si>
+  <si>
+    <t>students</t>
+  </si>
+  <si>
+    <t>taken</t>
+  </si>
+  <si>
+    <t>Viewed student details for student_id=301</t>
+  </si>
+  <si>
+    <t>Removed student_id=305 from course_id=201</t>
+  </si>
+  <si>
+    <t>Enrollment existed</t>
+  </si>
+  <si>
+    <t>1/4/2024  14:30:00 AM</t>
   </si>
 </sst>
 </file>
@@ -337,11 +401,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,9 +747,9 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -712,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -726,7 +791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -740,7 +805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -754,7 +819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -768,7 +833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -782,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -796,7 +861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -810,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -824,7 +889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -841,6 +906,150 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B71373-8C34-42E9-A897-97545D4EC0BC}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="12.25" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="2">
+        <v>45292.416666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="2">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -852,9 +1061,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +1077,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -882,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -896,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -923,9 +1132,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,7 +1148,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -953,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -967,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -994,9 +1203,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1024,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1038,7 +1247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1062,13 +1271,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9576CF3-E415-D74F-9078-D5FB5CF33D2D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1090,7 +1299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1101,7 +1310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1125,12 +1334,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1371,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1194,7 +1403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1226,7 +1435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1258,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1290,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1322,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1354,7 +1563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1386,7 +1595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1411,9 +1620,9 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1424,7 +1633,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1435,7 +1644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1446,7 +1655,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1457,7 +1666,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1468,7 +1677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1479,7 +1688,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1490,7 +1699,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1501,7 +1710,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1512,7 +1721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1523,7 +1732,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1534,7 +1743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1545,7 +1754,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1556,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1580,13 +1789,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1806,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1608,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1619,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1630,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1641,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1652,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1676,9 +1885,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1901,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1706,7 +1915,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Staff dashboard now has manage courses and assign instructors forms with courses and instructor tables.
</commit_message>
<xml_diff>
--- a/backend/temporaryData.xlsx
+++ b/backend/temporaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokt\Desktop\bloop2\eduPortal\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242AE6FB-8150-403A-AD19-395266BEE05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC8D0B7-EB89-47F1-8CBF-522B2D60CBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="9" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
   </bookViews>
   <sheets>
     <sheet name="student_data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -913,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B71373-8C34-42E9-A897-97545D4EC0BC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1328,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CED518-FDB6-C641-98AE-D7DBD2B33CA5}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1339,7 @@
     <col min="4" max="4" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1370,8 +1370,11 @@
       <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1402,8 +1405,11 @@
       <c r="J2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1434,8 +1440,11 @@
       <c r="J3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1466,8 +1475,11 @@
       <c r="J4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1498,8 +1510,11 @@
       <c r="J5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1530,8 +1545,11 @@
       <c r="J6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1562,8 +1580,11 @@
       <c r="J7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1594,8 +1615,11 @@
       <c r="J8" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>

</xml_diff>

<commit_message>
Added manage students and department student tables to Staff Dashboard.
</commit_message>
<xml_diff>
--- a/backend/temporaryData.xlsx
+++ b/backend/temporaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokt\Desktop\bloop2\eduPortal\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC8D0B7-EB89-47F1-8CBF-522B2D60CBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07811B3D-3AA3-4385-B791-25944136EB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
   </bookViews>
   <sheets>
     <sheet name="student_data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="157">
   <si>
     <t>id</t>
   </si>
@@ -360,6 +360,162 @@
   </si>
   <si>
     <t>1/4/2024  14:30:00 AM</t>
+  </si>
+  <si>
+    <t>instructor4</t>
+  </si>
+  <si>
+    <t>instructor5</t>
+  </si>
+  <si>
+    <t>instructor6</t>
+  </si>
+  <si>
+    <t>BUL</t>
+  </si>
+  <si>
+    <t>Law And Business I</t>
+  </si>
+  <si>
+    <t>CAI</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence and Business Analytics for Organizations</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>Principles of Finance</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>Principles of Management</t>
+  </si>
+  <si>
+    <t>QMB</t>
+  </si>
+  <si>
+    <t>Data Analytics for Business</t>
+  </si>
+  <si>
+    <t>RMI</t>
+  </si>
+  <si>
+    <t>Principles of Risk Management</t>
+  </si>
+  <si>
+    <t>Operations and Supply Chain Management</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>Geology</t>
+  </si>
+  <si>
+    <t>Photography</t>
+  </si>
+  <si>
+    <t>Astronomy</t>
+  </si>
+  <si>
+    <t>student11</t>
+  </si>
+  <si>
+    <t>student12</t>
+  </si>
+  <si>
+    <t>student13</t>
+  </si>
+  <si>
+    <t>student14</t>
+  </si>
+  <si>
+    <t>student15</t>
+  </si>
+  <si>
+    <t>student16</t>
+  </si>
+  <si>
+    <t>student17</t>
+  </si>
+  <si>
+    <t>pass17</t>
+  </si>
+  <si>
+    <t>pass11</t>
+  </si>
+  <si>
+    <t>pass12</t>
+  </si>
+  <si>
+    <t>pass13</t>
+  </si>
+  <si>
+    <t>pass14</t>
+  </si>
+  <si>
+    <t>pass15</t>
+  </si>
+  <si>
+    <t>pass16</t>
+  </si>
+  <si>
+    <t>advisor4</t>
+  </si>
+  <si>
+    <t>advisor5</t>
+  </si>
+  <si>
+    <t>staff4</t>
+  </si>
+  <si>
+    <t>staff5</t>
+  </si>
+  <si>
+    <t>GLY</t>
+  </si>
+  <si>
+    <t>Computational Geology</t>
+  </si>
+  <si>
+    <t>History of Life</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>Introduction Earth Science</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>Descriptive Astronomy</t>
+  </si>
+  <si>
+    <t>Stellar Astronomy and Cosmology</t>
+  </si>
+  <si>
+    <t>PGY</t>
+  </si>
+  <si>
+    <t>2401C</t>
+  </si>
+  <si>
+    <t>Beginning Photography</t>
+  </si>
+  <si>
+    <t>4420C</t>
+  </si>
+  <si>
+    <t>Advanced Photography</t>
   </si>
 </sst>
 </file>
@@ -741,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAE6502-C1FF-4442-9779-D2F2C733D118}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -901,6 +1057,104 @@
       </c>
       <c r="D11">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -914,7 +1168,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1055,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF79B0C-F0F0-7848-870C-E4A13F6EF13D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1119,6 +1373,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1126,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD49859-03EE-0D47-BC97-8E8CB56AF00A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1190,6 +1472,48 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1197,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23A5609-D1EF-4642-A90E-2DCFC0299B6D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1259,6 +1583,34 @@
       </c>
       <c r="D4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1328,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CED518-FDB6-C641-98AE-D7DBD2B33CA5}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1578,7 +1930,7 @@
         <v>72</v>
       </c>
       <c r="J7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1613,23 +1965,501 @@
         <v>68</v>
       </c>
       <c r="J8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3320</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3801</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3403</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3025</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3302</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3004</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4504</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3866</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2090</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="1">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="1">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="1">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1638,10 +2468,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4100F00-74C3-F34F-967E-137DAA4061B3}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1800,6 +2630,237 @@
         <v>4</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>18</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>19</v>
+      </c>
+      <c r="C33">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>3.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1807,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDB9195-415A-484E-BDE9-1D7DAA68536C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1896,6 +2957,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1903,10 +2997,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91206F6A-5B4C-234C-BF08-1B78D3E11924}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1953,6 +3047,20 @@
         <v>1001</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4">
+        <v>330</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added toggle to show passwords on manage students and manage instructors page. Still deciding whether to keep manage advisors as requirements have advisors many to many with departments.
</commit_message>
<xml_diff>
--- a/backend/temporaryData.xlsx
+++ b/backend/temporaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokt\Desktop\bloop2\eduPortal\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07811B3D-3AA3-4385-B791-25944136EB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55F55F6-3813-4DF9-81FC-F6AC18B486ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA2852CD-56E6-2A4F-96A4-989284897563}"/>
   </bookViews>
   <sheets>
     <sheet name="student_data" sheetId="1" r:id="rId1"/>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAE6502-C1FF-4442-9779-D2F2C733D118}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B71373-8C34-42E9-A897-97545D4EC0BC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2470,7 +2470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4100F00-74C3-F34F-967E-137DAA4061B3}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -2506,7 +2506,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>3.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>3.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>2.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>2.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>2.2999999999999998</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
         <v>13</v>
       </c>
       <c r="C19">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,7 +2770,7 @@
         <v>5</v>
       </c>
       <c r="C27">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2781,7 +2781,7 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>2.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2836,7 +2836,7 @@
         <v>19</v>
       </c>
       <c r="C33">
-        <v>3.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2858,7 +2858,7 @@
         <v>21</v>
       </c>
       <c r="C35">
-        <v>3.6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2870,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDB9195-415A-484E-BDE9-1D7DAA68536C}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>